<commit_message>
DDT added to ContactsUs for TC_OC_CU_003,004,005
</commit_message>
<xml_diff>
--- a/src/test/resources/ContactUsData.xlsx
+++ b/src/test/resources/ContactUsData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5551BF3-51ED-4B19-8200-D730045F3287}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5A5B9177-3BF8-4BC6-ADA2-314BEF5553CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3370" yWindow="1820" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="14430" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Errol</t>
   </si>
@@ -34,16 +30,49 @@
   </si>
   <si>
     <t>Testing if this field is working without</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>demo1@example</t>
+  </si>
+  <si>
+    <t>When will the iPad Air be in stock again</t>
+  </si>
+  <si>
+    <t>Te</t>
+  </si>
+  <si>
+    <t>demo1@example.com</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,13 +95,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -351,29 +384,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{B276759B-0DB4-458A-B606-54317CFE620C}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{73820A20-9A13-4FA7-9C83-1C5BD7E71E1B}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{45A5A84A-1472-466D-AE90-13CCF98F71F9}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{9C11C28A-2DAA-4EC5-B6A3-BF3330274B22}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>